<commit_message>
Add single row for editing
</commit_message>
<xml_diff>
--- a/Intervention evaluation study/Inputs/BCIO_Intervention_Evaluation_Study_Defs.xlsx
+++ b/Intervention evaluation study/Inputs/BCIO_Intervention_Evaluation_Study_Defs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\OneDrive\Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Intervention evaluation study/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8366E68E-16F9-40AF-9ACC-E6C15218AD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282EDBE4-EF47-FE40-95AE-877BB529BA99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -113,13 +113,25 @@
   </si>
   <si>
     <t>Reviewer comment</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Proposed</t>
+  </si>
+  <si>
+    <t>Please remove this row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,13 +478,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,16 +579,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -595,12 +611,16 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AE2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -633,7 +653,7 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -666,7 +686,7 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -699,7 +719,7 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -732,7 +752,7 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -765,7 +785,7 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -798,7 +818,7 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -831,7 +851,7 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -864,7 +884,7 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -897,7 +917,7 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -930,7 +950,7 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -963,7 +983,7 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -996,7 +1016,7 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1029,7 +1049,7 @@
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1062,7 +1082,7 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1095,7 +1115,7 @@
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1128,7 +1148,7 @@
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1161,7 +1181,7 @@
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1194,7 +1214,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1227,7 +1247,7 @@
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1260,7 +1280,7 @@
       <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1293,7 +1313,7 @@
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1326,7 +1346,7 @@
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1359,7 +1379,7 @@
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1392,7 +1412,7 @@
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1425,7 +1445,7 @@
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1458,7 +1478,7 @@
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1491,7 +1511,7 @@
       <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1524,7 +1544,7 @@
       <c r="AD33" s="2"/>
       <c r="AE33" s="2"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1557,7 +1577,7 @@
       <c r="AD34" s="2"/>
       <c r="AE34" s="2"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1590,7 +1610,7 @@
       <c r="AD36" s="2"/>
       <c r="AE36" s="2"/>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1623,7 +1643,7 @@
       <c r="AD37" s="2"/>
       <c r="AE37" s="2"/>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1656,7 +1676,7 @@
       <c r="AD38" s="2"/>
       <c r="AE38" s="2"/>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1689,7 +1709,7 @@
       <c r="AD40" s="2"/>
       <c r="AE40" s="2"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1722,7 +1742,7 @@
       <c r="AD41" s="2"/>
       <c r="AE41" s="2"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1755,7 +1775,7 @@
       <c r="AD42" s="2"/>
       <c r="AE42" s="2"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1788,7 +1808,7 @@
       <c r="AD43" s="2"/>
       <c r="AE43" s="2"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1821,7 +1841,7 @@
       <c r="AD44" s="2"/>
       <c r="AE44" s="2"/>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1854,7 +1874,7 @@
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1887,7 +1907,7 @@
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1920,7 +1940,7 @@
       <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1953,7 +1973,7 @@
       <c r="AD48" s="2"/>
       <c r="AE48" s="2"/>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:31">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -1986,7 +2006,7 @@
       <c r="AD49" s="2"/>
       <c r="AE49" s="2"/>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:31">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2019,7 +2039,7 @@
       <c r="AD50" s="2"/>
       <c r="AE50" s="2"/>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:31">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2052,7 +2072,7 @@
       <c r="AD51" s="2"/>
       <c r="AE51" s="2"/>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:31">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2085,7 +2105,7 @@
       <c r="AD52" s="2"/>
       <c r="AE52" s="2"/>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:31">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2118,7 +2138,7 @@
       <c r="AD53" s="2"/>
       <c r="AE53" s="2"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:31">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2151,7 +2171,7 @@
       <c r="AD54" s="2"/>
       <c r="AE54" s="2"/>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:31">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2184,7 +2204,7 @@
       <c r="AD55" s="2"/>
       <c r="AE55" s="2"/>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:31">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2217,7 +2237,7 @@
       <c r="AD56" s="2"/>
       <c r="AE56" s="2"/>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:31">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2250,7 +2270,7 @@
       <c r="AD57" s="2"/>
       <c r="AE57" s="2"/>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:31">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>

</xml_diff>